<commit_message>
Update report and research
</commit_message>
<xml_diff>
--- a/Course project/research/23_clean.xlsx
+++ b/Course project/research/23_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmitr\Desktop\6 сем\матстат\PolyMatStat\Course project\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17A111E-4861-4839-92B2-E2B1FA64717B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308439E3-E768-407A-8FF9-B84CEE2CFF68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -579,7 +580,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>